<commit_message>
- Added GetColumn and GetRow funxtions on worksheet - Removed similar functions from the WorksheetReader - Added test for the WorksheetReader
</commit_message>
<xml_diff>
--- a/NanoXlsx Test/Resources/tampered.xlsx
+++ b/NanoXlsx Test/Resources/tampered.xlsx
@@ -82,6 +82,12 @@
       <c r="H1" t="z">
         <v>y</v>
       </c>
+      <c r="I1" t="b">
+        <v>true</v>
+      </c>
+      <c r="J1" t="b">
+        <v>FALSE</v>
+      </c>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
Adapted handling of malformed files; Added tests
</commit_message>
<xml_diff>
--- a/NanoXlsx Test/Resources/tampered.xlsx
+++ b/NanoXlsx Test/Resources/tampered.xlsx
@@ -67,10 +67,10 @@
       <c r="C1" s="2">
         <v>-1.8538541667</v>
       </c>
-      <c t="b" r="D1" s="2">
+      <c t="b" r="D1">
         <v>2</v>
       </c>
-      <c t="b" r="E1" s="2">
+      <c t="b" r="E1">
         <v>x</v>
       </c>
       <c t="s" r="F1">

</xml_diff>